<commit_message>
Phone Masking and Db Clear
1. Clear Database Functionality
2. Phone Masking
</commit_message>
<xml_diff>
--- a/Timesheets/kjohnson6.xlsx
+++ b/Timesheets/kjohnson6.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Senior Project - Spring / Summer 2015</t>
   </si>
@@ -50,6 +50,24 @@
   </si>
   <si>
     <t>Code Cleanup</t>
+  </si>
+  <si>
+    <t>05/27/2015 Wed</t>
+  </si>
+  <si>
+    <t>1:15pm-4:00pm</t>
+  </si>
+  <si>
+    <t>Class Meeting, Team Meeting, Debugging</t>
+  </si>
+  <si>
+    <t>05/28/2015 Thu</t>
+  </si>
+  <si>
+    <t>4:45pm-</t>
+  </si>
+  <si>
+    <t>SRS Document Revision,</t>
   </si>
 </sst>
 </file>
@@ -221,7 +239,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -291,16 +309,30 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>

</xml_diff>